<commit_message>
Feature/download work is true,task5 download score id->nickname
</commit_message>
<xml_diff>
--- a/common/util/task5score.xlsx
+++ b/common/util/task5score.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21030" windowHeight="10610"/>
+    <workbookView windowHeight="17810"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <t>任务名字</t>
   </si>
   <si>
-    <t>咨询师ID</t>
+    <t>咨询师</t>
   </si>
   <si>
     <t>能准确识别风险并提出转介建议</t>
@@ -1393,15 +1393,15 @@
   <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.22727272727273" defaultRowHeight="14" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="3" width="13.4545454545455" customWidth="1"/>
     <col min="4" max="12" width="30.7636363636364" style="3" customWidth="1"/>
-    <col min="13" max="13" width="13.4545454545455" customWidth="1"/>
+    <col min="13" max="13" width="20.0545454545455" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="68" customHeight="1" spans="1:13">

</xml_diff>